<commit_message>
Add example of how to avoid divide by zero in UDT
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_udt.xlsx
+++ b/tests/frameworks/framework_udt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856D55B4-37EB-4148-BDBB-92568660A169}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C9A438-4F29-4AED-B1B9-DDBCACD09A0E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -1048,24 +1048,15 @@
     <t>num_diag</t>
   </si>
   <si>
-    <t>num_diag/undx</t>
-  </si>
-  <si>
     <t>num_initiate</t>
   </si>
   <si>
     <t>Initiation rate</t>
   </si>
   <si>
-    <t>num_initiate/dx</t>
-  </si>
-  <si>
     <t>num_loss</t>
   </si>
   <si>
-    <t>num_loss/tx</t>
-  </si>
-  <si>
     <t>Annual number of new diagnoses</t>
   </si>
   <si>
@@ -1085,6 +1076,15 @@
   </si>
   <si>
     <t>UDT example</t>
+  </si>
+  <si>
+    <t>num_loss/max(tx,num_loss)</t>
+  </si>
+  <si>
+    <t>num_initiate/max(dx,num_initiate)</t>
+  </si>
+  <si>
+    <t>num_diag/max(undx,num_diag)</t>
   </si>
 </sst>
 </file>
@@ -1516,7 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41729878-D668-43BB-8A23-5831FD580C69}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1524,18 +1524,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1620,7 +1620,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="166" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1745,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1801,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,7 +1931,7 @@
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1977,7 +1977,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>42</v>
@@ -2017,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>8</v>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>42</v>
@@ -2062,7 +2062,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -2075,7 +2075,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>8</v>
@@ -2090,10 +2090,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>42</v>
@@ -2133,7 +2133,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>8</v>

</xml_diff>